<commit_message>
doc (work logs) : update
Updating the work logs
</commit_message>
<xml_diff>
--- a/T-CraftMeUp_JonathanJunod.xlsx
+++ b/T-CraftMeUp_JonathanJunod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe40boh\Documents\GitHub\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{D876CB4B-008E-4333-BE47-174DAD3A224E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{49C3D4D1-FA8C-4A30-8C9B-417FD5D42074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -167,10 +167,25 @@
     <t>24p</t>
   </si>
   <si>
-    <t>INF / portes ouvertes / -</t>
-  </si>
-  <si>
     <t>Craft Me Up, un jeu en winforms pour les portes ouvertes</t>
+  </si>
+  <si>
+    <t>INF / DEV / P_Prod</t>
+  </si>
+  <si>
+    <t>Class diagram</t>
+  </si>
+  <si>
+    <t>Creating a diagram for the code's classes</t>
+  </si>
+  <si>
+    <t>Explanations</t>
+  </si>
+  <si>
+    <t>Explanations of the code for me</t>
+  </si>
+  <si>
+    <t>https://eduvaud-my.sharepoint.com/:u:/r/personal/pb62kjx_eduvaud_ch/_layouts/15/Doc.aspx?sourcedoc=%7B5BF0A89E-E3A6-4CD4-BA7E-BFDC17A68BD3%7D&amp;file=P_CraftMeUp_ClassDiagram.vsdx&amp;fromShare=true&amp;action=default&amp;mobileredirect=true</t>
   </si>
 </sst>
 </file>
@@ -918,7 +933,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -981,7 +996,7 @@
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="33"/>
     </row>
@@ -990,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -1029,38 +1044,60 @@
         <v>45964</v>
       </c>
       <c r="C6" s="5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="37">
-        <v>0.58680555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="B7" s="24"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="22"/>
+      <c r="C7" s="7">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="37">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="B8" s="24"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="19"/>
+      <c r="C8" s="7">
+        <v>45</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="37">
+        <v>0.65625</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
@@ -1092,7 +1129,7 @@
       </c>
       <c r="D11" s="34">
         <f>SUM(C6:C10)</f>
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
@@ -1546,7 +1583,7 @@
       <c r="B54" s="27"/>
       <c r="C54" s="12">
         <f>MROUND(SUM(C6:C53) /60,0.2)</f>
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="18"/>
@@ -1591,7 +1628,7 @@
     <mergeCell ref="B42:B46"/>
     <mergeCell ref="B48:B52"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C48:C52 C36:C40 C42:C46 C18:C22 B6 C12:C16 C24:C28 C30:C34 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
@@ -1622,7 +1659,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E10 A12:E16 A18:E22 A24:E28 A30:E34 A36:E40 A42:E46 A48:E52 A54:E1048576 A1:D3 F1:F3 G4:G10 A11:D11 A17:D17 A23:D23 A29:D29 A35:D35 A41:D41 A47:D47 A53:D53 G54:G1048576</xm:sqref>
+          <xm:sqref>A12:E16 A18:E22 A24:E28 A30:E34 A36:E40 A42:E46 A48:E52 A54:E1048576 A1:D3 F1:F3 G4:G10 A11:D11 A17:D17 A23:D23 A29:D29 A35:D35 A41:D41 A47:D47 A53:D53 G54:G1048576 A4:E6 B7:C7 E7 A8:E10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="11" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -1775,7 +1812,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E11ED1A-D9E7-4F6F-A32A-17EE6B774A99}">
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>

</xml_diff>

<commit_message>
doc (work logs) : updating
</commit_message>
<xml_diff>
--- a/T-CraftMeUp_JonathanJunod.xlsx
+++ b/T-CraftMeUp_JonathanJunod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe40boh\Documents\GitHub\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9576ADC9-0FD6-46F1-AA62-C7E1494D755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2039DEDB-E2CA-47CA-AD70-10DD1F1CE2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>https://github.com/users/Jonathan150408/projects/6/views/1</t>
+  </si>
+  <si>
+    <t>Updating the classes diagram</t>
+  </si>
+  <si>
+    <t>Correcting Shoot me up</t>
+  </si>
+  <si>
+    <t>Optimizing Shoot me up</t>
   </si>
 </sst>
 </file>
@@ -523,6 +532,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -531,44 +576,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -976,7 +985,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -996,65 +1005,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1083,7 +1092,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="25">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1106,7 +1115,7 @@
       <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1125,7 +1134,7 @@
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="7">
         <v>45</v>
       </c>
@@ -1152,13 +1161,13 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="36">
         <f>SUM(C6:C8)</f>
         <v>110</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1191,19 +1200,19 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="36">
         <f>SUM(C10:C10)</f>
         <v>30</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="25">
         <v>45971</v>
       </c>
       <c r="C12" s="5">
@@ -1224,7 +1233,7 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7">
         <v>5</v>
       </c>
@@ -1245,7 +1254,7 @@
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="7">
         <v>10</v>
       </c>
@@ -1264,7 +1273,7 @@
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="7">
         <v>50</v>
       </c>
@@ -1283,7 +1292,7 @@
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="9">
         <v>25</v>
       </c>
@@ -1310,44 +1319,76 @@
       <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="36">
         <f>SUM(C12:C16)</f>
         <v>135</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="22"/>
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="25">
+        <v>45978</v>
+      </c>
+      <c r="C18" s="5">
+        <v>15</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0.55902777777777779</v>
+      </c>
       <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="22"/>
+      <c r="A19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="7">
+        <v>105</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="24">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="7">
+        <v>25</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0.64236111111111105</v>
+      </c>
       <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="31"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1356,7 +1397,7 @@
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
-      <c r="B22" s="32"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="9"/>
       <c r="D22" s="8"/>
       <c r="E22" s="10"/>
@@ -1373,17 +1414,17 @@
       <c r="C23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="36">
         <f>SUM(C18:C22)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+        <v>145</v>
+      </c>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="30"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="5"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1392,7 +1433,7 @@
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="31"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1401,7 +1442,7 @@
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="31"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1410,7 +1451,7 @@
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="31"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1419,7 +1460,7 @@
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
-      <c r="B28" s="32"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="9"/>
       <c r="D28" s="8"/>
       <c r="E28" s="10"/>
@@ -1436,17 +1477,17 @@
       <c r="C29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="36">
         <f>SUM(C24:C28)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="30"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="5"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1455,7 +1496,7 @@
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="31"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1464,7 +1505,7 @@
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="31"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1473,7 +1514,7 @@
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="31"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -1482,7 +1523,7 @@
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
-      <c r="B34" s="32"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="9"/>
       <c r="D34" s="8"/>
       <c r="E34" s="10"/>
@@ -1499,17 +1540,17 @@
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="36">
         <f>SUM(C30:C34)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="30"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="5"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1518,7 +1559,7 @@
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="31"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1527,7 +1568,7 @@
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="31"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="7"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -1536,7 +1577,7 @@
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="31"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -1545,7 +1586,7 @@
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
-      <c r="B40" s="32"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="9"/>
       <c r="D40" s="8"/>
       <c r="E40" s="10"/>
@@ -1562,17 +1603,17 @@
       <c r="C41" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="36">
         <f>SUM(C36:C40)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="30"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="5"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -1581,7 +1622,7 @@
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="31"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -1590,7 +1631,7 @@
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="31"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -1599,7 +1640,7 @@
     </row>
     <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="31"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -1608,7 +1649,7 @@
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
-      <c r="B46" s="32"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="9"/>
       <c r="D46" s="8"/>
       <c r="E46" s="10"/>
@@ -1625,22 +1666,22 @@
       <c r="C47" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="25">
+      <c r="D47" s="36">
         <f>SUM(C42:C46)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="38"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="12">
         <f>MROUND(SUM(C6:C47) /60,0.2)</f>
-        <v>4.6000000000000005</v>
+        <v>7</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="18"/>
@@ -1657,12 +1698,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B16"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1672,17 +1718,12 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B42:B46"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C42:C46 C30:C34 C36:C40 C12:C16 B6 C10 C18:C22 C24:C28 C6:C8" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1715,7 +1756,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E22 A24:E28 A30:E34 A36:E40 A42:E46 A48:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 A23:D23 A29:D29 A35:D35 A41:D41 A47:D47 G48:G1048576</xm:sqref>
+          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A24:E28 A30:E34 A36:E40 A42:E46 A48:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 A23:D23 A29:D29 A35:D35 A41:D41 A47:D47 G48:G1048576 A18:E18 A21:E22 A19:C19 A20:D20 E19:E20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="11" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -1909,26 +1950,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2171,10 +2192,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2191,20 +2243,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(work logs) : updating
</commit_message>
<xml_diff>
--- a/T-CraftMeUp_JonathanJunod.xlsx
+++ b/T-CraftMeUp_JonathanJunod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe40boh\Documents\GitHub\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55311CDA-8B3A-4AD7-AE7F-7F5F6984CE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAB986-9757-49C4-B792-D8C74E6AC764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Restrictions" sheetId="19" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$45</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>Implementing the new random wave generation</t>
+  </si>
+  <si>
+    <t>Implementing the random wave generation system</t>
+  </si>
+  <si>
+    <t>trying to fix the memory leak</t>
   </si>
 </sst>
 </file>
@@ -553,6 +559,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -561,44 +603,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -993,13 +999,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1019,65 +1025,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1106,7 +1112,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="25">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1129,7 +1135,7 @@
       <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1148,7 +1154,7 @@
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="7">
         <v>45</v>
       </c>
@@ -1175,13 +1181,13 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="36">
         <f>SUM(C6:C8)</f>
         <v>110</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1214,19 +1220,19 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="36">
         <f>SUM(C10:C10)</f>
         <v>30</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="25">
         <v>45971</v>
       </c>
       <c r="C12" s="5">
@@ -1247,7 +1253,7 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7">
         <v>5</v>
       </c>
@@ -1268,7 +1274,7 @@
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="7">
         <v>10</v>
       </c>
@@ -1287,7 +1293,7 @@
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="7">
         <v>50</v>
       </c>
@@ -1306,7 +1312,7 @@
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="9">
         <v>25</v>
       </c>
@@ -1333,19 +1339,19 @@
       <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="36">
         <f>SUM(C12:C16)</f>
         <v>135</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="25">
         <v>45978</v>
       </c>
       <c r="C18" s="5">
@@ -1366,7 +1372,7 @@
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="7">
         <v>105</v>
       </c>
@@ -1385,7 +1391,7 @@
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="7">
         <v>25</v>
       </c>
@@ -1410,19 +1416,19 @@
       <c r="C21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="36">
         <f>SUM(C18:C20)</f>
         <v>145</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="25">
         <v>45985</v>
       </c>
       <c r="C22" s="5">
@@ -1445,7 +1451,7 @@
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="31"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="7">
         <v>80</v>
       </c>
@@ -1464,7 +1470,7 @@
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="7">
         <v>5</v>
       </c>
@@ -1479,11 +1485,11 @@
       </c>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="7">
         <v>20</v>
       </c>
@@ -1499,99 +1505,123 @@
       <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="19"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B26" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="25">
-        <f>SUM(C22:C26)</f>
+      <c r="D26" s="36">
+        <f>SUM(C22:C25)</f>
         <v>145</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="25">
+        <v>45992</v>
+      </c>
+      <c r="C27" s="5">
+        <v>35</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="24">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="19"/>
+      <c r="A28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="7">
+        <v>105</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="24">
+        <v>0.65625</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="31"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="22"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="31"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="7"/>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="7"/>
+    <row r="31" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="7"/>
       <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="19"/>
-    </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="A32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B32" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="25">
-        <f>SUM(C28:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="D32" s="36">
+        <f>SUM(C27:C31)</f>
+        <v>140</v>
+      </c>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="5"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="22"/>
@@ -1599,62 +1629,62 @@
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="31"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="22"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="31"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="7"/>
       <c r="G36" s="19"/>
     </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="7"/>
+    <row r="37" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="7"/>
       <c r="G37" s="19"/>
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="19"/>
-    </row>
-    <row r="39" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
+      <c r="A38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B38" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C38" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="25">
-        <f>SUM(C34:C38)</f>
+      <c r="D38" s="36">
+        <f>SUM(C33:C37)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
+    </row>
+    <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="5"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="22"/>
@@ -1662,88 +1692,84 @@
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="31"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="22"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="19"/>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="31"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="7"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="7"/>
       <c r="G42" s="19"/>
     </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="7"/>
+    <row r="43" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
       <c r="F43" s="7"/>
       <c r="G43" s="19"/>
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="45" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B44" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="25">
-        <f>SUM(C40:C44)</f>
+      <c r="D44" s="36">
+        <f>SUM(C39:C43)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
-    </row>
-    <row r="46" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="37"/>
+    </row>
+    <row r="45" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="12">
-        <f>MROUND(SUM(C6:C45) /60,0.2)</f>
-        <v>9.4</v>
-      </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="14"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="12">
+        <f>MROUND(SUM(C6:C44) /60,0.2)</f>
+        <v>11.8</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A47" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B16"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1753,34 +1779,32 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="B39:B43"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C40:C44 C28:C32 C34:C38 C12:C16 B6 C10 C22:C26 C6:C8 C18:C20" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C39:C43 C27:C31 C33:C37 C12:C16 B6 C10 C22:C25 C6:C8 C18:C20" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B26 B28:B32 B34:B38 B40:B44 B18:B20" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B25 B27:B31 B33:B37 B39:B43 B18:B20" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G28" r:id="rId1" xr:uid="{16D500E2-F10E-4EDF-9AB5-CBC9CC38D0A3}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1796,7 +1820,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E26 A28:E32 A34:E38 A40:E44 A46:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 A19:C19 A20:D21 A27:D27 A33:D33 A39:D39 A45:D45 G46:G1048576 F18:G20</xm:sqref>
+          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E25 A27:E31 A33:E37 A39:E43 A45:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 F18:G20 A19:C19 A20:D21 A26:D26 A32:D32 A38:D38 A44:D44 G45:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="11" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -1832,7 +1856,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E8 E10 E12:E16 E22:E26 E28:E32 E34:E38 E40:E44 E46:E1048576 E18:E20</xm:sqref>
+          <xm:sqref>E4:E8 E10 E12:E16 E18:E20 E22:E25 E27:E31 E33:E37 E39:E43 E45:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -1888,11 +1912,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F22:G26</xm:sqref>
+          <xm:sqref>F22:G25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F28)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F27)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1902,11 +1926,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F28:G32</xm:sqref>
+          <xm:sqref>F27:G31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F34)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F33)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1916,11 +1940,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F34:G38</xm:sqref>
+          <xm:sqref>F33:G37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F40)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F39)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1930,7 +1954,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F40:G44</xm:sqref>
+          <xm:sqref>F39:G43</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1940,7 +1964,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E26 E28:E32 E34:E38 E40:E44 E46:E1048576 E18:E20</xm:sqref>
+          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E25 E27:E31 E33:E37 E39:E43 E45:E1048576 E18:E20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1976,26 +2000,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2238,10 +2242,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2258,20 +2293,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc ( work logs) : updating the work logs
</commit_message>
<xml_diff>
--- a/T-CraftMeUp_JonathanJunod.xlsx
+++ b/T-CraftMeUp_JonathanJunod.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe40boh\Documents\GitHub\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAB986-9757-49C4-B792-D8C74E6AC764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2854D41-A9B9-464C-A3BC-6DA5AA5F5EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
     <sheet name="Restrictions" sheetId="19" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$42</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -261,6 +261,27 @@
   </si>
   <si>
     <t>trying to fix the memory leak</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>I was supposed to go to Sebeillon but actually not</t>
+  </si>
+  <si>
+    <t>installation</t>
+  </si>
+  <si>
+    <t>Installing visual studio 2026</t>
+  </si>
+  <si>
+    <t>implementing the bosses waves for later (no bosses now)</t>
+  </si>
+  <si>
+    <t>Implementing the pause menu</t>
+  </si>
+  <si>
+    <t>fixing the broken wave generation</t>
   </si>
 </sst>
 </file>
@@ -559,6 +580,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -571,40 +609,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,13 +1020,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1025,65 +1046,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="35"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="35"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1112,7 +1133,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="30">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1135,7 +1156,7 @@
       <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1154,7 +1175,7 @@
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="7">
         <v>45</v>
       </c>
@@ -1181,13 +1202,13 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="25">
         <f>SUM(C6:C8)</f>
         <v>110</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1220,19 +1241,19 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="25">
         <f>SUM(C10:C10)</f>
         <v>30</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="30">
         <v>45971</v>
       </c>
       <c r="C12" s="5">
@@ -1253,7 +1274,7 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="7">
         <v>5</v>
       </c>
@@ -1274,7 +1295,7 @@
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="7">
         <v>10</v>
       </c>
@@ -1293,7 +1314,7 @@
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="7">
         <v>50</v>
       </c>
@@ -1312,7 +1333,7 @@
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="9">
         <v>25</v>
       </c>
@@ -1339,19 +1360,19 @@
       <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="25">
         <f>SUM(C12:C16)</f>
         <v>135</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="30">
         <v>45978</v>
       </c>
       <c r="C18" s="5">
@@ -1372,7 +1393,7 @@
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="7">
         <v>105</v>
       </c>
@@ -1391,7 +1412,7 @@
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="7">
         <v>25</v>
       </c>
@@ -1416,19 +1437,19 @@
       <c r="C21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="25">
         <f>SUM(C18:C20)</f>
         <v>145</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="30">
         <v>45985</v>
       </c>
       <c r="C22" s="5">
@@ -1451,7 +1472,7 @@
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="7">
         <v>80</v>
       </c>
@@ -1470,7 +1491,7 @@
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="7">
         <v>5</v>
       </c>
@@ -1489,7 +1510,7 @@
       <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="7">
         <v>20</v>
       </c>
@@ -1514,19 +1535,19 @@
       <c r="C26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="25">
         <f>SUM(C22:C25)</f>
         <v>145</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="30">
         <v>45992</v>
       </c>
       <c r="C27" s="5">
@@ -1543,11 +1564,11 @@
       </c>
       <c r="G27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="7">
         <v>105</v>
       </c>
@@ -1564,212 +1585,232 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="19"/>
+    <row r="29" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="25">
+        <f>SUM(C27:C28)</f>
+        <v>140</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="30">
+        <v>45999</v>
+      </c>
+      <c r="C30" s="5">
+        <v>25</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="24">
+        <v>0.35069444444444442</v>
+      </c>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="7"/>
+    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="7">
+        <v>35</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0.375</v>
+      </c>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="7">
+        <v>25</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="24">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="7">
+        <v>45</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="32"/>
+      <c r="C34" s="9">
+        <v>15</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="17" t="s">
+      <c r="B35" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="36">
-        <f>SUM(C27:C31)</f>
-        <v>140</v>
-      </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="37"/>
-    </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="19"/>
+      <c r="D35" s="25">
+        <f>SUM(C30:C34)</f>
+        <v>145</v>
+      </c>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="19"/>
     </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="9"/>
+    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="19"/>
     </row>
-    <row r="38" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="36">
-        <f>SUM(C33:C37)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="37"/>
+    <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="19"/>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="22"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="19"/>
     </row>
-    <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="7"/>
+    <row r="40" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="19"/>
     </row>
-    <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="19"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="19"/>
-    </row>
-    <row r="44" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+    <row r="41" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B41" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C41" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="36">
-        <f>SUM(C39:C43)</f>
+      <c r="D41" s="25">
+        <f>SUM(C36:C40)</f>
         <v>0</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="37"/>
-    </row>
-    <row r="45" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="28" t="s">
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
+    </row>
+    <row r="42" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="12">
-        <f>MROUND(SUM(C6:C44) /60,0.2)</f>
-        <v>11.8</v>
-      </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="14"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="B42" s="38"/>
+      <c r="C42" s="12">
+        <f>MROUND(SUM(C6:C41) /60,0.2)</f>
+        <v>14.200000000000001</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B36:B40"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1779,18 +1820,23 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D41:G41"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C39:C43 C27:C31 C33:C37 C12:C16 B6 C10 C22:C25 C6:C8 C18:C20" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C36:C40 C27:C28 C30:C34 C12:C16 B6 C10 C22:C25 C6:C8 C18:C20" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B25 B27:B31 B33:B37 B39:B43 B18:B20" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B25 B27:B28 B30:B34 B36:B40 B18:B20" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1820,7 +1866,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E25 A27:E31 A33:E37 A39:E43 A45:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 F18:G20 A19:C19 A20:D21 A26:D26 A32:D32 A38:D38 A44:D44 G45:G1048576</xm:sqref>
+          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E25 A27:E28 A30:E34 A36:E40 A42:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 F18:G20 A19:C19 A20:D21 A26:D26 A29:D29 A35:D35 A41:D41 G42:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="11" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
@@ -1856,7 +1902,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E8 E10 E12:E16 E18:E20 E22:E25 E27:E31 E33:E37 E39:E43 E45:E1048576</xm:sqref>
+          <xm:sqref>E4:E8 E10 E12:E16 E18:E20 E22:E25 E27:E28 E30:E34 E36:E40 E42:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
@@ -1926,11 +1972,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F27:G31</xm:sqref>
+          <xm:sqref>F27:G28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F33)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F30)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1940,11 +1986,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F33:G37</xm:sqref>
+          <xm:sqref>F30:G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
-            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F39)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F36)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1954,7 +2000,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F39:G43</xm:sqref>
+          <xm:sqref>F36:G40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1964,7 +2010,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E25 E27:E31 E33:E37 E39:E43 E45:E1048576 E18:E20</xm:sqref>
+          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E25 E27:E28 E30:E34 E36:E40 E42:E1048576 E18:E20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2000,6 +2046,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2242,27 +2308,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2279,23 +2344,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc (work log) : update
</commit_message>
<xml_diff>
--- a/T-CraftMeUp_JonathanJunod.xlsx
+++ b/T-CraftMeUp_JonathanJunod.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pe40boh\Documents\GitHub\Craft-Me-Up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2854D41-A9B9-464C-A3BC-6DA5AA5F5EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FC63F5-F5A1-4F43-B9A0-DF4F9E25A94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
     <sheet name="Restrictions" sheetId="19" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$54</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -283,12 +283,42 @@
   <si>
     <t>fixing the broken wave generation</t>
   </si>
+  <si>
+    <t>Jour 9</t>
+  </si>
+  <si>
+    <t>Jour 10</t>
+  </si>
+  <si>
+    <t>Work at home</t>
+  </si>
+  <si>
+    <t>Installing visual studio 2026 om the usual pc</t>
+  </si>
+  <si>
+    <t>Correcting</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Making the evaluation of my project with M. Mveng</t>
+  </si>
+  <si>
+    <t>Correcting the rapport of my mysql project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding </t>
+  </si>
+  <si>
+    <t>Waiting fr Neo to be done, helping him</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -324,6 +354,11 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -493,7 +528,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -588,15 +623,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -605,6 +631,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -621,18 +653,89 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1020,13 +1123,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1046,65 +1149,65 @@
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1133,7 +1236,7 @@
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="27">
         <v>45964</v>
       </c>
       <c r="C6" s="5">
@@ -1156,7 +1259,7 @@
       <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="7">
         <v>35</v>
       </c>
@@ -1175,7 +1278,7 @@
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="7">
         <v>45</v>
       </c>
@@ -1202,13 +1305,13 @@
       <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="38">
         <f>SUM(C6:C8)</f>
         <v>110</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1229,7 +1332,9 @@
       <c r="F10" s="24">
         <v>0.68055555555555547</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="41" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
@@ -1241,19 +1346,19 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="38">
         <f>SUM(C10:C10)</f>
         <v>30</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="27">
         <v>45971</v>
       </c>
       <c r="C12" s="5">
@@ -1274,7 +1379,7 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7">
         <v>5</v>
       </c>
@@ -1295,7 +1400,7 @@
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="7">
         <v>10</v>
       </c>
@@ -1314,7 +1419,7 @@
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="7">
         <v>50</v>
       </c>
@@ -1333,7 +1438,7 @@
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="9">
         <v>25</v>
       </c>
@@ -1360,19 +1465,19 @@
       <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="38">
         <f>SUM(C12:C16)</f>
         <v>135</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="27">
         <v>45978</v>
       </c>
       <c r="C18" s="5">
@@ -1393,7 +1498,7 @@
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="7">
         <v>105</v>
       </c>
@@ -1412,7 +1517,7 @@
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="7">
         <v>25</v>
       </c>
@@ -1437,19 +1542,19 @@
       <c r="C21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="38">
         <f>SUM(C18:C20)</f>
         <v>145</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="27">
         <v>45985</v>
       </c>
       <c r="C22" s="5">
@@ -1472,7 +1577,7 @@
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="31"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="7">
         <v>80</v>
       </c>
@@ -1491,7 +1596,7 @@
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="7">
         <v>5</v>
       </c>
@@ -1510,7 +1615,7 @@
       <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="7">
         <v>20</v>
       </c>
@@ -1535,19 +1640,19 @@
       <c r="C26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="38">
         <f>SUM(C22:C25)</f>
         <v>145</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="27">
         <v>45992</v>
       </c>
       <c r="C27" s="5">
@@ -1568,7 +1673,7 @@
       <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="7">
         <v>105</v>
       </c>
@@ -1595,19 +1700,19 @@
       <c r="C29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="38">
         <f>SUM(C27:C28)</f>
         <v>140</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="27">
         <v>45999</v>
       </c>
       <c r="C30" s="5">
@@ -1628,7 +1733,7 @@
       <c r="A31" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="31"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="7">
         <v>35</v>
       </c>
@@ -1647,7 +1752,7 @@
       <c r="A32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="31"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="7">
         <v>25</v>
       </c>
@@ -1666,7 +1771,7 @@
       <c r="A33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="7">
         <v>45</v>
       </c>
@@ -1685,7 +1790,7 @@
       <c r="A34" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="32"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="9">
         <v>15</v>
       </c>
@@ -1710,57 +1815,109 @@
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="38">
         <f>SUM(C30:C34)</f>
         <v>145</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="22"/>
+      <c r="A36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="27">
+        <v>46006</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="24">
+        <v>0.55208333333333337</v>
+      </c>
       <c r="G36" s="19"/>
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="22"/>
+      <c r="A37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="7">
+        <v>25</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="24">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="G37" s="19"/>
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
+      <c r="A38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="28"/>
+      <c r="C38" s="7">
+        <v>45</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="24">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="G38" s="19"/>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="7">
+        <v>35</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="24">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="7"/>
+      <c r="A40" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="31"/>
+      <c r="C40" s="9">
+        <v>30</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0.65625</v>
+      </c>
       <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1775,42 +1932,172 @@
       </c>
       <c r="D41" s="25">
         <f>SUM(C36:C40)</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
+    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="25">
+        <f>SUM(C42:C46)</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="26"/>
+    </row>
+    <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="19"/>
+    </row>
+    <row r="52" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="25">
+        <f>SUM(C48:C52)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
+    </row>
+    <row r="54" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="12">
+      <c r="B54" s="30"/>
+      <c r="C54" s="12">
         <f>MROUND(SUM(C6:C41) /60,0.2)</f>
-        <v>14.200000000000001</v>
-      </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B36:B40"/>
+  <mergeCells count="27">
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B16"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -1820,23 +2107,20 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B42:B46"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C36:C40 C27:C28 C30:C34 C12:C16 B6 C10 C22:C25 C6:C8 C18:C20" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C18:C20 C27:C28 C30:C34 C12:C16 B6 C10 C22:C25 C6:C8 C36:C40 C42:C46 C48:C52" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B25 B27:B28 B30:B34 B36:B40 B18:B20" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B10 B12:B16 B22:B25 B27:B28 B30:B34 B18:B20 B42 B48 B36" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1855,7 +2139,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{57C84C53-B905-437D-BEEF-7124C39AA062}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,A1)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1866,10 +2150,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E25 A27:E28 A30:E34 A36:E40 A42:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 F18:G20 A19:C19 A20:D21 A26:D26 A29:D29 A35:D35 A41:D41 G42:G1048576</xm:sqref>
+          <xm:sqref>A4:E6 E7 A8:E8 A10:E10 A12:E16 A18:E18 E19:E20 A22:E25 A27:E28 A30:E34 A36:E36 A54:E1048576 A1:D3 F1:F3 G4:G8 B7:C7 A9:D9 A11:D11 A17:D17 F18:G20 A19:C19 A20:D21 A26:D26 A29:D29 A35:D35 A41:D41 G54:G1048576 A42:E42 A47:D47 A48:E48 A53:D53 A49:A52 C49:E52 A43:A46 C43:E46 A37:A38 A40 C37:E38 C39 E39 C40:E40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="endsWith" priority="11" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
+          <x14:cfRule type="endsWith" priority="19" operator="endsWith" id="{FA4647AC-51FE-4597-AE79-DF1EBCADBA52}">
             <xm:f>RIGHT(E4,LEN(Restrictions!$A$1))=Restrictions!$A$1</xm:f>
             <xm:f>Restrictions!$A$1</xm:f>
             <x14:dxf>
@@ -1880,7 +2164,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{CA908F4B-0D6A-49FA-81F5-C1AAB26EE444}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$C$1,E4)))</xm:f>
             <xm:f>Restrictions!$C$1</xm:f>
             <x14:dxf>
@@ -1891,7 +2175,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{BC07C843-4761-4226-B9B3-580ED2061AC2}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$D$1,E4)))</xm:f>
             <xm:f>Restrictions!$D$1</xm:f>
             <x14:dxf>
@@ -1902,10 +2186,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4:E8 E10 E12:E16 E18:E20 E22:E25 E27:E28 E30:E34 E36:E40 E42:E1048576</xm:sqref>
+          <xm:sqref>E4:E8 E10 E12:E16 E18:E20 E22:E25 E27:E28 E30:E34 E36:E40 E54:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{FD0F452B-B2F8-4F75-A8CD-A69AC0834E64}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F6)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1919,7 +2203,7 @@
           <xm:sqref>F6:F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{88417B48-EA26-4D48-9EFE-B6A1E5C426AE}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{88417B48-EA26-4D48-9EFE-B6A1E5C426AE}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F10)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1933,7 +2217,7 @@
           <xm:sqref>F10:G10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{6407061A-B268-44CE-A52C-133739941B16}">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{6407061A-B268-44CE-A52C-133739941B16}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F12)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1947,7 +2231,7 @@
           <xm:sqref>F12:G16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{E988FD75-2909-4816-91C7-1018002A435D}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F22)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1961,7 +2245,7 @@
           <xm:sqref>F22:G25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{D5B6D5DF-9E2A-4C4B-BA82-97D983766AEE}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F27)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1975,7 +2259,7 @@
           <xm:sqref>F27:G28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{1555D56B-E8B5-4F0A-9D80-B2C1016EB105}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F30)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -1989,7 +2273,7 @@
           <xm:sqref>F30:G34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{2F0F41F7-8C93-48A6-B013-C45F8E29AE34}">
             <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F36)))</xm:f>
             <xm:f>Restrictions!$B$1</xm:f>
             <x14:dxf>
@@ -2002,6 +2286,106 @@
           </x14:cfRule>
           <xm:sqref>F36:G40</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="endsWith" priority="6" operator="endsWith" id="{0824E982-851B-43C9-93B9-AD66F1F6D9D3}">
+            <xm:f>RIGHT(E42,LEN(Restrictions!$A$1))=Restrictions!$A$1</xm:f>
+            <xm:f>Restrictions!$A$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{DAC71B9F-704A-4AC1-91D2-AA157FC6C941}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$C$1,E42)))</xm:f>
+            <xm:f>Restrictions!$C$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{8CD92D65-DB99-48C3-817C-584F5DCFC949}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$D$1,E42)))</xm:f>
+            <xm:f>Restrictions!$D$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E42:E46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{B54B1C5A-0B7C-448A-BE0F-9080E524C8FF}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F42)))</xm:f>
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F42:G46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="endsWith" priority="2" operator="endsWith" id="{6BD03225-AC35-4EF8-9778-8E33BBCD2312}">
+            <xm:f>RIGHT(E48,LEN(Restrictions!$A$1))=Restrictions!$A$1</xm:f>
+            <xm:f>Restrictions!$A$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{B31645C9-5C3F-46FD-8679-03B668B2A898}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$C$1,E48)))</xm:f>
+            <xm:f>Restrictions!$C$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{366832FF-CB44-44C1-A820-1FEC74D360A4}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$D$1,E48)))</xm:f>
+            <xm:f>Restrictions!$D$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E48:E52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{DB2561A6-E98C-40A3-A9DD-B3F8BB3F76A0}">
+            <xm:f>NOT(ISERROR(SEARCH(Restrictions!$B$1,F48)))</xm:f>
+            <xm:f>Restrictions!$B$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F48:G52</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2010,7 +2394,7 @@
           <x14:formula1>
             <xm:f>Restrictions!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E25 E27:E28 E30:E34 E36:E40 E42:E1048576 E18:E20</xm:sqref>
+          <xm:sqref>E1:E4 E6:E8 E10 E12:E16 E22:E25 E27:E28 E30:E34 E18:E20 E54:E1048576 E36:E40 E42:E46 E48:E52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2046,26 +2430,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2308,10 +2672,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a1b10758-7132-46a4-a2fe-7a2cf46f51f4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2328,20 +2723,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>